<commit_message>
N3 e input contrato itaquera no material.
</commit_message>
<xml_diff>
--- a/MateriaisContratada.xlsx
+++ b/MateriaisContratada.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20398"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{387FE5D2-A5AF-49CD-A211-25844F8F0740}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30479323-8684-41DD-A9F5-016F72011550}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>50000017</t>
   </si>
@@ -122,6 +122,30 @@
   </si>
   <si>
     <t>30007737</t>
+  </si>
+  <si>
+    <t>30000732</t>
+  </si>
+  <si>
+    <t>COTOVELO 90 GR PVC JS DN 20 (DR 15 MM)</t>
+  </si>
+  <si>
+    <t>50000333</t>
+  </si>
+  <si>
+    <t>PORCA PVC BRANCA DN 20</t>
+  </si>
+  <si>
+    <t>30003758</t>
+  </si>
+  <si>
+    <t>TE PVC JS DN 20 X 20</t>
+  </si>
+  <si>
+    <t>30000880</t>
+  </si>
+  <si>
+    <t>TUBO PVC RIGIDO PB JS DN 25 (DR 20 MM)</t>
   </si>
 </sst>
 </file>
@@ -445,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,129 +491,161 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>